<commit_message>
census data and coordinating stuff
coordinating color across different icicle views
basic checkbox functionality for adding all exporters
basic view of census poverty data now available in viewer
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>tasks</t>
   </si>
@@ -111,6 +111,24 @@
   </si>
   <si>
     <t>put icicile into callback queue</t>
+  </si>
+  <si>
+    <t>footer: data update, sources</t>
+  </si>
+  <si>
+    <t>info panel : census data</t>
+  </si>
+  <si>
+    <t>mess with changing symbology of waste sites: no color</t>
+  </si>
+  <si>
+    <t>description of the site after "Welcome to Haz Mat Mapper"</t>
+  </si>
+  <si>
+    <t>add show all exporters/importers checkboxes to filter menu</t>
+  </si>
+  <si>
+    <t>create color key to coordinate site color across icicle, map, and pov chart</t>
   </si>
 </sst>
 </file>
@@ -160,10 +178,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,19 +614,64 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>